<commit_message>
changed color of waveForms
</commit_message>
<xml_diff>
--- a/SampleAudioWaveformPaths.xlsx
+++ b/SampleAudioWaveformPaths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NoteBook\Desktop\programing\Data Science\Uni project\final project\MahdyMokh7-Speech-Emotion-Recognition-en-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A60D6E-B98D-4336-A1C8-2D919FCDBFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA74508-EB21-48AD-9B8D-0A02709D4A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Fear</t>
   </si>
   <si>
-    <t>Surprise</t>
-  </si>
-  <si>
     <t>Disgust</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/MahdyMokh7/MahdyMokh7-Speech-Emotion-Recognition-en-/master/sampleAudios/1052_ITS_HAP_XX.wav</t>
+  </si>
+  <si>
+    <t>Neutral</t>
   </si>
 </sst>
 </file>
@@ -937,7 +937,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,21 +962,21 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -984,10 +984,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -995,32 +995,32 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>